<commit_message>
More work on JPADCore_v2 and JPADCore in order to run a complete aircraft analysis.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/IRON/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/IRON/WEIGHTS/Weights.xlsx
@@ -1564,7 +1564,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>970.2</v>
+        <v>2233.0999999999995</v>
       </c>
     </row>
     <row r="3">
@@ -1599,7 +1599,7 @@
         <v>1679.0</v>
       </c>
       <c r="D6" t="n">
-        <v>73.05710162853019</v>
+        <v>-24.81304016837578</v>
       </c>
     </row>
     <row r="7">
@@ -1613,7 +1613,7 @@
         <v>2351.0</v>
       </c>
       <c r="D7" t="n">
-        <v>142.32117089259947</v>
+        <v>5.2796560834714334</v>
       </c>
     </row>
     <row r="8">
@@ -1627,7 +1627,7 @@
         <v>2690.0</v>
       </c>
       <c r="D8" t="n">
-        <v>177.26242011956296</v>
+        <v>20.460346603376504</v>
       </c>
     </row>
     <row r="9">
@@ -1641,7 +1641,7 @@
         <v>2318.0</v>
       </c>
       <c r="D9" t="n">
-        <v>138.91981034838176</v>
+        <v>3.8018897496753645</v>
       </c>
     </row>
     <row r="10">

</xml_diff>